<commit_message>
working random names python
</commit_message>
<xml_diff>
--- a/Project Files/Words.xlsx
+++ b/Project Files/Words.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="205">
   <si>
     <t>Letters</t>
   </si>
@@ -625,6 +625,15 @@
   </si>
   <si>
     <t>Addon Objects +</t>
+  </si>
+  <si>
+    <t>Queen Latifah</t>
+  </si>
+  <si>
+    <t>Velociraptor</t>
+  </si>
+  <si>
+    <t>Xmen</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1075,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,6 +1593,9 @@
       <c r="A18" s="13" t="s">
         <v>128</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>129</v>
       </c>
@@ -1705,6 +1717,9 @@
       <c r="A23" s="13" t="s">
         <v>158</v>
       </c>
+      <c r="B23" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="F23" s="14" t="s">
         <v>159</v>
       </c>
@@ -1744,6 +1759,9 @@
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>168</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>169</v>

</xml_diff>